<commit_message>
Changed DHT22 sensor locations
</commit_message>
<xml_diff>
--- a/mega_datalogger/mega_pinouts.xlsx
+++ b/mega_datalogger/mega_pinouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\GitHub\GreenhouseHVAC\mega_datalogger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C938A212-3F3F-4183-8481-6D11599E44FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E743FC2B-BD51-4571-8F38-DD4EC77BA326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="1875" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{613FAFC2-106D-4226-818B-E16DFC4791C8}"/>
+    <workbookView xWindow="22365" yWindow="4980" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{613FAFC2-106D-4226-818B-E16DFC4791C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinouts" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="108">
   <si>
     <t>GND</t>
   </si>
@@ -341,10 +341,16 @@
     <t>sensors</t>
   </si>
   <si>
-    <t>Removed, DHT22 can't be placed more than 1m out</t>
-  </si>
-  <si>
     <t>removed DHT22 cannot be placed past 1m</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>DHT33</t>
   </si>
 </sst>
 </file>
@@ -400,10 +406,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D7E0061-D64D-44EA-BC0C-D42A4DD10076}">
-  <dimension ref="A2:E97"/>
+  <dimension ref="A2:H97"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,9 +737,10 @@
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -748,33 +756,36 @@
       <c r="E2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -788,37 +799,37 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -922,60 +933,25 @@
       <c r="A32">
         <v>22</v>
       </c>
-      <c r="B32" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>23</v>
       </c>
-      <c r="B33" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D33" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>24</v>
       </c>
-      <c r="B34" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D34" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>25</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>104</v>
-      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
@@ -986,21 +962,54 @@
       <c r="A37">
         <v>27</v>
       </c>
+      <c r="B37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>28</v>
       </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>29</v>
       </c>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>30</v>
       </c>
+      <c r="B40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" t="s">
+        <v>101</v>
+      </c>
       <c r="D40" t="s">
         <v>57</v>
       </c>
@@ -1120,7 +1129,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>39</v>
       </c>
@@ -1133,8 +1142,14 @@
       <c r="D49" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>1.5</v>
+      </c>
+      <c r="H49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>40</v>
       </c>
@@ -1147,8 +1162,11 @@
       <c r="D50" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>41</v>
       </c>
@@ -1164,8 +1182,11 @@
       <c r="E51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>42</v>
       </c>
@@ -1181,8 +1202,11 @@
       <c r="E52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>43</v>
       </c>
@@ -1198,8 +1222,11 @@
       <c r="E53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>44</v>
       </c>
@@ -1215,8 +1242,11 @@
       <c r="E54" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>45</v>
       </c>
@@ -1232,8 +1262,11 @@
       <c r="E55" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>46</v>
       </c>
@@ -1247,7 +1280,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>47</v>
       </c>
@@ -1255,37 +1288,37 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -1483,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50295567-E213-4C52-ABA6-F26FF9EEE0BC}">
   <dimension ref="A3:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,38 +1967,36 @@
       <c r="A43" t="s">
         <v>96</v>
       </c>
-      <c r="B43">
-        <v>22</v>
-      </c>
       <c r="C43" t="s">
         <v>97</v>
       </c>
+      <c r="D43">
+        <v>27</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <v>23</v>
-      </c>
       <c r="C44" t="s">
         <v>98</v>
       </c>
+      <c r="D44">
+        <v>28</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>24</v>
-      </c>
       <c r="C45" t="s">
         <v>99</v>
       </c>
+      <c r="D45">
+        <v>29</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="2">
-        <v>25</v>
-      </c>
+      <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
         <v>100</v>
       </c>
       <c r="D46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>